<commit_message>
<feat>(all):Correction Dictionnaire et MCD
</commit_message>
<xml_diff>
--- a/Dictionnaire de données.xlsx
+++ b/Dictionnaire de données.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="41">
   <si>
     <t>Utilisateur</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Propriétés</t>
+  </si>
+  <si>
+    <t>Niveau</t>
   </si>
 </sst>
 </file>
@@ -542,7 +545,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,12 +776,12 @@
       <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -789,23 +792,21 @@
       <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E16" s="8"/>
+      <c r="F16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -816,21 +817,16 @@
       <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="7"/>
-      <c r="F19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>8</v>
+    </row>
+    <row r="19" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -844,11 +840,11 @@
         <v>6</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>21</v>
+      <c r="F20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -861,10 +857,10 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -875,12 +871,12 @@
       <c r="C22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -891,6 +887,13 @@
       <c r="C23" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
@@ -899,6 +902,13 @@
       </c>
       <c r="C24" s="3" t="s">
         <v>27</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>